<commit_message>
Convert all v1 to v2
</commit_message>
<xml_diff>
--- a/tools/excel/adobe/adobe-ccf-v5.xlsx
+++ b/tools/excel/adobe/adobe-ccf-v5.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="library_content" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="requirements" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="answers" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="library_meta" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="requirements_meta" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="requirements_content" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="answers_meta" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="answers_content" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,192 +428,121 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>library_urn</t>
+          <t>type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>urn:intuitem:risk:library:adobe-ccf-v5</t>
+          <t>library</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>library_version</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
+          <t>urn</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>urn:intuitem:risk:library:adobe-ccf-v5</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>library_locale</t>
+          <t>version</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>library_ref_id</t>
+          <t>locale</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>adobe-ccf-v5</t>
+          <t>en</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>library_name</t>
+          <t>ref_id</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Adobe CCF v5</t>
+          <t>adobe-ccf-v5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>library_description</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adobe Common Controls Framework (CCF) version 5
-https://www.adobe.com/trust/compliance/adobe-ccf.html
-</t>
+          <t>Adobe CCF v5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>library_copyright</t>
+          <t>description</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Creative Commons</t>
+          <t>Adobe Common Controls Framework (CCF) version 5
+https://www.adobe.com/trust/compliance/adobe-ccf.html</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>library_provider</t>
+          <t>copyright</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Adobe</t>
+          <t>Creative Commons</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>library_packager</t>
+          <t>provider</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>intuitem</t>
+          <t>Adobe</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>framework_urn</t>
+          <t>packager</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:intuitem:risk:framework:adobe-ccf-v5</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>framework_ref_id</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>adobe-ccf-v5</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>framework_name</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Adobe CCF v5</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>framework_description</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Adobe Common Controls Framework (CCF) version 5
-https://www.adobe.com/trust/compliance/adobe-ccf.html
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>tab</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>requirements</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>requirements</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>tab</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>answers</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>answers</t>
+          <t>intuitem</t>
         </is>
       </c>
     </row>
@@ -621,6 +552,110 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>framework</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>base_urn</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>urn:intuitem:risk:req_node:adobe-ccf-v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>urn</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>urn:intuitem:risk:framework:adobe-ccf-v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ref_id</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>adobe-ccf-v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Adobe CCF v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Adobe Common Controls Framework (CCF) version 5
+https://www.adobe.com/trust/compliance/adobe-ccf.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>answers_definition</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>answers</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -682,18 +717,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>Asset Management</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1333,18 +1364,14 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
       <c r="B16" t="n">
         <v>1</v>
       </c>
-      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
           <t>Business Continuity</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1642,18 +1669,14 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
       <c r="B23" t="n">
         <v>1</v>
       </c>
-      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
           <t>Backup Management</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1898,18 +1921,14 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
       <c r="B29" t="n">
         <v>1</v>
       </c>
-      <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
           <t>Configuration Management</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2669,18 +2688,14 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
       <c r="B45" t="n">
         <v>1</v>
       </c>
-      <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
           <t>Change Management</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2897,18 +2912,14 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr"/>
       <c r="B50" t="n">
         <v>1</v>
       </c>
-      <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
           <t>Customer Managed Security</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3102,18 +3113,14 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr"/>
       <c r="B55" t="n">
         <v>1</v>
       </c>
-      <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
           <t>Cryptography</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3864,18 +3871,14 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr"/>
       <c r="B71" t="n">
         <v>1</v>
       </c>
-      <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
           <t>Data Management</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4955,18 +4958,14 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr"/>
       <c r="B94" t="n">
         <v>1</v>
       </c>
-      <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr">
         <is>
           <t>Entity Management</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr"/>
-      <c r="F94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5510,18 +5509,14 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr"/>
       <c r="B106" t="n">
         <v>1</v>
       </c>
-      <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr">
         <is>
           <t>Identity and Access Management</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -7461,18 +7456,14 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr"/>
       <c r="B146" t="n">
         <v>1</v>
       </c>
-      <c r="C146" t="inlineStr"/>
       <c r="D146" t="inlineStr">
         <is>
           <t>Incident Response</t>
         </is>
       </c>
-      <c r="E146" t="inlineStr"/>
-      <c r="F146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -7925,18 +7916,14 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr"/>
       <c r="B155" t="n">
         <v>1</v>
       </c>
-      <c r="C155" t="inlineStr"/>
       <c r="D155" t="inlineStr">
         <is>
           <t>Mobile Device Management</t>
         </is>
       </c>
-      <c r="E155" t="inlineStr"/>
-      <c r="F155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -8135,18 +8122,14 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr"/>
       <c r="B160" t="n">
         <v>1</v>
       </c>
-      <c r="C160" t="inlineStr"/>
       <c r="D160" t="inlineStr">
         <is>
           <t>Network Operations</t>
         </is>
       </c>
-      <c r="E160" t="inlineStr"/>
-      <c r="F160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -9034,18 +9017,14 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr"/>
       <c r="B179" t="n">
         <v>1</v>
       </c>
-      <c r="C179" t="inlineStr"/>
       <c r="D179" t="inlineStr">
         <is>
           <t>People Resources</t>
         </is>
       </c>
-      <c r="E179" t="inlineStr"/>
-      <c r="F179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -9551,18 +9530,14 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="inlineStr"/>
       <c r="B190" t="n">
         <v>1</v>
       </c>
-      <c r="C190" t="inlineStr"/>
       <c r="D190" t="inlineStr">
         <is>
           <t>Privacy</t>
         </is>
       </c>
-      <c r="E190" t="inlineStr"/>
-      <c r="F190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -10057,18 +10032,14 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="inlineStr"/>
       <c r="B201" t="n">
         <v>1</v>
       </c>
-      <c r="C201" t="inlineStr"/>
       <c r="D201" t="inlineStr">
         <is>
           <t>Proactive Security</t>
         </is>
       </c>
-      <c r="E201" t="inlineStr"/>
-      <c r="F201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -10259,18 +10230,14 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="inlineStr"/>
       <c r="B206" t="n">
         <v>1</v>
       </c>
-      <c r="C206" t="inlineStr"/>
       <c r="D206" t="inlineStr">
         <is>
           <t>Risk Management</t>
         </is>
       </c>
-      <c r="E206" t="inlineStr"/>
-      <c r="F206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -10788,18 +10755,14 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" t="inlineStr"/>
       <c r="B217" t="n">
         <v>1</v>
       </c>
-      <c r="C217" t="inlineStr"/>
       <c r="D217" t="inlineStr">
         <is>
           <t>System Design Documentation</t>
         </is>
       </c>
-      <c r="E217" t="inlineStr"/>
-      <c r="F217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -10895,18 +10858,14 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" t="inlineStr"/>
       <c r="B220" t="n">
         <v>1</v>
       </c>
-      <c r="C220" t="inlineStr"/>
       <c r="D220" t="inlineStr">
         <is>
           <t>Security Governance</t>
         </is>
       </c>
-      <c r="E220" t="inlineStr"/>
-      <c r="F220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -11731,18 +11690,14 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" t="inlineStr"/>
       <c r="B238" t="n">
         <v>1</v>
       </c>
-      <c r="C238" t="inlineStr"/>
       <c r="D238" t="inlineStr">
         <is>
           <t>Service Lifecycle</t>
         </is>
       </c>
-      <c r="E238" t="inlineStr"/>
-      <c r="F238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -12101,18 +12056,14 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr"/>
       <c r="B246" t="n">
         <v>1</v>
       </c>
-      <c r="C246" t="inlineStr"/>
       <c r="D246" t="inlineStr">
         <is>
           <t>Systems Monitoring</t>
         </is>
       </c>
-      <c r="E246" t="inlineStr"/>
-      <c r="F246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -13785,18 +13736,14 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" t="inlineStr"/>
       <c r="B279" t="n">
         <v>1</v>
       </c>
-      <c r="C279" t="inlineStr"/>
       <c r="D279" t="inlineStr">
         <is>
           <t>Site Operations</t>
         </is>
       </c>
-      <c r="E279" t="inlineStr"/>
-      <c r="F279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -14587,18 +14534,14 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" t="inlineStr"/>
       <c r="B296" t="n">
         <v>1</v>
       </c>
-      <c r="C296" t="inlineStr"/>
       <c r="D296" t="inlineStr">
         <is>
           <t>Training and Awareness</t>
         </is>
       </c>
-      <c r="E296" t="inlineStr"/>
-      <c r="F296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -15055,18 +14998,14 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" t="inlineStr"/>
       <c r="B306" t="n">
         <v>1</v>
       </c>
-      <c r="C306" t="inlineStr"/>
       <c r="D306" t="inlineStr">
         <is>
           <t>Third-Party Management</t>
         </is>
       </c>
-      <c r="E306" t="inlineStr"/>
-      <c r="F306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -15712,18 +15651,14 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" t="inlineStr"/>
       <c r="B320" t="n">
         <v>1</v>
       </c>
-      <c r="C320" t="inlineStr"/>
       <c r="D320" t="inlineStr">
         <is>
           <t>Vulnerability Management</t>
         </is>
       </c>
-      <c r="E320" t="inlineStr"/>
-      <c r="F320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -16906,7 +16841,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>answers</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>answers</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
fix(lib): Convert all v1 Excel to v2 Format (#3492)
* Add Bulk Mode to "convert_v1_to_v2.py"

* Add "--old-output-dir" in order to separate v1 from v2 in Bulk mode

* Add "--output-suffix" parameter in order to add a suffix to output file

* Unmerge Cells

* Final Update Convert v1 to v2

* Extra tools

* Convert all v1 to v2
</commit_message>
<xml_diff>
--- a/tools/excel/adobe/adobe-ccf-v5.xlsx
+++ b/tools/excel/adobe/adobe-ccf-v5.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="library_content" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="requirements" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="answers" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="library_meta" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="requirements_meta" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="requirements_content" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="answers_meta" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="answers_content" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,192 +428,121 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>library_urn</t>
+          <t>type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>urn:intuitem:risk:library:adobe-ccf-v5</t>
+          <t>library</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>library_version</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
+          <t>urn</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>urn:intuitem:risk:library:adobe-ccf-v5</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>library_locale</t>
+          <t>version</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>library_ref_id</t>
+          <t>locale</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>adobe-ccf-v5</t>
+          <t>en</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>library_name</t>
+          <t>ref_id</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Adobe CCF v5</t>
+          <t>adobe-ccf-v5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>library_description</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adobe Common Controls Framework (CCF) version 5
-https://www.adobe.com/trust/compliance/adobe-ccf.html
-</t>
+          <t>Adobe CCF v5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>library_copyright</t>
+          <t>description</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Creative Commons</t>
+          <t>Adobe Common Controls Framework (CCF) version 5
+https://www.adobe.com/trust/compliance/adobe-ccf.html</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>library_provider</t>
+          <t>copyright</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Adobe</t>
+          <t>Creative Commons</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>library_packager</t>
+          <t>provider</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>intuitem</t>
+          <t>Adobe</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>framework_urn</t>
+          <t>packager</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:intuitem:risk:framework:adobe-ccf-v5</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>framework_ref_id</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>adobe-ccf-v5</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>framework_name</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Adobe CCF v5</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>framework_description</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Adobe Common Controls Framework (CCF) version 5
-https://www.adobe.com/trust/compliance/adobe-ccf.html
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>tab</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>requirements</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>requirements</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>tab</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>answers</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>answers</t>
+          <t>intuitem</t>
         </is>
       </c>
     </row>
@@ -621,6 +552,110 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>framework</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>base_urn</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>urn:intuitem:risk:req_node:adobe-ccf-v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>urn</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>urn:intuitem:risk:framework:adobe-ccf-v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ref_id</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>adobe-ccf-v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Adobe CCF v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Adobe Common Controls Framework (CCF) version 5
+https://www.adobe.com/trust/compliance/adobe-ccf.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>answers_definition</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>answers</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -682,18 +717,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>Asset Management</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1333,18 +1364,14 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
       <c r="B16" t="n">
         <v>1</v>
       </c>
-      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
           <t>Business Continuity</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1642,18 +1669,14 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
       <c r="B23" t="n">
         <v>1</v>
       </c>
-      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
           <t>Backup Management</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1898,18 +1921,14 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
       <c r="B29" t="n">
         <v>1</v>
       </c>
-      <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
           <t>Configuration Management</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2669,18 +2688,14 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
       <c r="B45" t="n">
         <v>1</v>
       </c>
-      <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
           <t>Change Management</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2897,18 +2912,14 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr"/>
       <c r="B50" t="n">
         <v>1</v>
       </c>
-      <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
           <t>Customer Managed Security</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3102,18 +3113,14 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr"/>
       <c r="B55" t="n">
         <v>1</v>
       </c>
-      <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
           <t>Cryptography</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3864,18 +3871,14 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr"/>
       <c r="B71" t="n">
         <v>1</v>
       </c>
-      <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
           <t>Data Management</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4955,18 +4958,14 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr"/>
       <c r="B94" t="n">
         <v>1</v>
       </c>
-      <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr">
         <is>
           <t>Entity Management</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr"/>
-      <c r="F94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5510,18 +5509,14 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr"/>
       <c r="B106" t="n">
         <v>1</v>
       </c>
-      <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr">
         <is>
           <t>Identity and Access Management</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -7461,18 +7456,14 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr"/>
       <c r="B146" t="n">
         <v>1</v>
       </c>
-      <c r="C146" t="inlineStr"/>
       <c r="D146" t="inlineStr">
         <is>
           <t>Incident Response</t>
         </is>
       </c>
-      <c r="E146" t="inlineStr"/>
-      <c r="F146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -7925,18 +7916,14 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr"/>
       <c r="B155" t="n">
         <v>1</v>
       </c>
-      <c r="C155" t="inlineStr"/>
       <c r="D155" t="inlineStr">
         <is>
           <t>Mobile Device Management</t>
         </is>
       </c>
-      <c r="E155" t="inlineStr"/>
-      <c r="F155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -8135,18 +8122,14 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr"/>
       <c r="B160" t="n">
         <v>1</v>
       </c>
-      <c r="C160" t="inlineStr"/>
       <c r="D160" t="inlineStr">
         <is>
           <t>Network Operations</t>
         </is>
       </c>
-      <c r="E160" t="inlineStr"/>
-      <c r="F160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -9034,18 +9017,14 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr"/>
       <c r="B179" t="n">
         <v>1</v>
       </c>
-      <c r="C179" t="inlineStr"/>
       <c r="D179" t="inlineStr">
         <is>
           <t>People Resources</t>
         </is>
       </c>
-      <c r="E179" t="inlineStr"/>
-      <c r="F179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -9551,18 +9530,14 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="inlineStr"/>
       <c r="B190" t="n">
         <v>1</v>
       </c>
-      <c r="C190" t="inlineStr"/>
       <c r="D190" t="inlineStr">
         <is>
           <t>Privacy</t>
         </is>
       </c>
-      <c r="E190" t="inlineStr"/>
-      <c r="F190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -10057,18 +10032,14 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="inlineStr"/>
       <c r="B201" t="n">
         <v>1</v>
       </c>
-      <c r="C201" t="inlineStr"/>
       <c r="D201" t="inlineStr">
         <is>
           <t>Proactive Security</t>
         </is>
       </c>
-      <c r="E201" t="inlineStr"/>
-      <c r="F201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -10259,18 +10230,14 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="inlineStr"/>
       <c r="B206" t="n">
         <v>1</v>
       </c>
-      <c r="C206" t="inlineStr"/>
       <c r="D206" t="inlineStr">
         <is>
           <t>Risk Management</t>
         </is>
       </c>
-      <c r="E206" t="inlineStr"/>
-      <c r="F206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -10788,18 +10755,14 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" t="inlineStr"/>
       <c r="B217" t="n">
         <v>1</v>
       </c>
-      <c r="C217" t="inlineStr"/>
       <c r="D217" t="inlineStr">
         <is>
           <t>System Design Documentation</t>
         </is>
       </c>
-      <c r="E217" t="inlineStr"/>
-      <c r="F217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -10895,18 +10858,14 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" t="inlineStr"/>
       <c r="B220" t="n">
         <v>1</v>
       </c>
-      <c r="C220" t="inlineStr"/>
       <c r="D220" t="inlineStr">
         <is>
           <t>Security Governance</t>
         </is>
       </c>
-      <c r="E220" t="inlineStr"/>
-      <c r="F220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -11731,18 +11690,14 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" t="inlineStr"/>
       <c r="B238" t="n">
         <v>1</v>
       </c>
-      <c r="C238" t="inlineStr"/>
       <c r="D238" t="inlineStr">
         <is>
           <t>Service Lifecycle</t>
         </is>
       </c>
-      <c r="E238" t="inlineStr"/>
-      <c r="F238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -12101,18 +12056,14 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr"/>
       <c r="B246" t="n">
         <v>1</v>
       </c>
-      <c r="C246" t="inlineStr"/>
       <c r="D246" t="inlineStr">
         <is>
           <t>Systems Monitoring</t>
         </is>
       </c>
-      <c r="E246" t="inlineStr"/>
-      <c r="F246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -13785,18 +13736,14 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" t="inlineStr"/>
       <c r="B279" t="n">
         <v>1</v>
       </c>
-      <c r="C279" t="inlineStr"/>
       <c r="D279" t="inlineStr">
         <is>
           <t>Site Operations</t>
         </is>
       </c>
-      <c r="E279" t="inlineStr"/>
-      <c r="F279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -14587,18 +14534,14 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" t="inlineStr"/>
       <c r="B296" t="n">
         <v>1</v>
       </c>
-      <c r="C296" t="inlineStr"/>
       <c r="D296" t="inlineStr">
         <is>
           <t>Training and Awareness</t>
         </is>
       </c>
-      <c r="E296" t="inlineStr"/>
-      <c r="F296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -15055,18 +14998,14 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" t="inlineStr"/>
       <c r="B306" t="n">
         <v>1</v>
       </c>
-      <c r="C306" t="inlineStr"/>
       <c r="D306" t="inlineStr">
         <is>
           <t>Third-Party Management</t>
         </is>
       </c>
-      <c r="E306" t="inlineStr"/>
-      <c r="F306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -15712,18 +15651,14 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" t="inlineStr"/>
       <c r="B320" t="n">
         <v>1</v>
       </c>
-      <c r="C320" t="inlineStr"/>
       <c r="D320" t="inlineStr">
         <is>
           <t>Vulnerability Management</t>
         </is>
       </c>
-      <c r="E320" t="inlineStr"/>
-      <c r="F320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -16906,7 +16841,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>answers</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>answers</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>